<commit_message>
Graph analysis base on record data
</commit_message>
<xml_diff>
--- a/User_record.xlsx
+++ b/User_record.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Rafi\all codes\Python Project\Entry Form wih Qr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Rafi\all codes\Python Project\EntryRecord\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99214D02-225A-4844-BA08-C79DFC7FE6F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7CD369C-0D02-4BE2-92F6-53640B633ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11627,8 +11627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView tabSelected="1" topLeftCell="A357" workbookViewId="0">
+      <selection activeCell="C386" sqref="C386"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -12508,7 +12508,7 @@
         <v>117</v>
       </c>
       <c r="C16">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
         <v>70</v>
@@ -12917,7 +12917,7 @@
         <v>154</v>
       </c>
       <c r="C23">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="D23" t="s">
         <v>48</v>
@@ -13092,7 +13092,7 @@
         <v>169</v>
       </c>
       <c r="C26">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="D26" t="s">
         <v>70</v>
@@ -13149,7 +13149,7 @@
         <v>175</v>
       </c>
       <c r="C27">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D27" t="s">
         <v>70</v>
@@ -14419,7 +14419,7 @@
         <v>286</v>
       </c>
       <c r="C49">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="D49" t="s">
         <v>70</v>
@@ -14765,7 +14765,7 @@
         <v>316</v>
       </c>
       <c r="C55" s="4">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D55" t="s">
         <v>70</v>
@@ -15456,7 +15456,7 @@
         <v>376</v>
       </c>
       <c r="C67">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="D67" t="s">
         <v>48</v>
@@ -15688,7 +15688,7 @@
         <v>396</v>
       </c>
       <c r="C71">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D71" t="s">
         <v>48</v>
@@ -15863,7 +15863,7 @@
         <v>411</v>
       </c>
       <c r="C74">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="D74" t="s">
         <v>48</v>
@@ -15881,7 +15881,7 @@
         <v>414</v>
       </c>
       <c r="I74" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J74" t="s">
         <v>79</v>
@@ -15979,7 +15979,7 @@
         <v>421</v>
       </c>
       <c r="C76">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="D76" t="s">
         <v>70</v>
@@ -15997,7 +15997,7 @@
         <v>389</v>
       </c>
       <c r="I76" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J76" t="s">
         <v>43</v>
@@ -16092,7 +16092,7 @@
         <v>430</v>
       </c>
       <c r="C78">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="D78" t="s">
         <v>48</v>
@@ -16149,7 +16149,7 @@
         <v>435</v>
       </c>
       <c r="C79">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D79" t="s">
         <v>48</v>
@@ -16167,7 +16167,7 @@
         <v>438</v>
       </c>
       <c r="I79" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J79" t="s">
         <v>105</v>
@@ -16558,7 +16558,7 @@
         <v>470</v>
       </c>
       <c r="C86">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D86" t="s">
         <v>48</v>
@@ -16794,7 +16794,7 @@
         <v>490</v>
       </c>
       <c r="C90" s="4">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="D90" t="s">
         <v>48</v>
@@ -17026,7 +17026,7 @@
         <v>510</v>
       </c>
       <c r="C94">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D94" t="s">
         <v>48</v>
@@ -17044,7 +17044,7 @@
         <v>513</v>
       </c>
       <c r="I94" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J94" t="s">
         <v>105</v>
@@ -17142,7 +17142,7 @@
         <v>520</v>
       </c>
       <c r="C96">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D96" t="s">
         <v>48</v>
@@ -17431,7 +17431,7 @@
         <v>545</v>
       </c>
       <c r="C101" s="4">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="D101" t="s">
         <v>48</v>
@@ -17488,7 +17488,7 @@
         <v>550</v>
       </c>
       <c r="C102" s="4">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D102" t="s">
         <v>48</v>
@@ -17889,7 +17889,7 @@
         <v>585</v>
       </c>
       <c r="C109">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="D109" t="s">
         <v>48</v>
@@ -17907,7 +17907,7 @@
         <v>588</v>
       </c>
       <c r="I109" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J109" t="s">
         <v>86</v>
@@ -18297,7 +18297,7 @@
         <v>619</v>
       </c>
       <c r="C116">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="D116" t="s">
         <v>48</v>
@@ -18315,7 +18315,7 @@
         <v>622</v>
       </c>
       <c r="I116" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J116" t="s">
         <v>173</v>
@@ -18356,7 +18356,7 @@
         <v>624</v>
       </c>
       <c r="C117">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="D117" t="s">
         <v>48</v>
@@ -18642,7 +18642,7 @@
         <v>649</v>
       </c>
       <c r="C122" s="4">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="D122" t="s">
         <v>48</v>
@@ -18660,7 +18660,7 @@
         <v>652</v>
       </c>
       <c r="I122" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J122" t="s">
         <v>79</v>
@@ -18868,7 +18868,7 @@
         <v>669</v>
       </c>
       <c r="C126">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="D126" t="s">
         <v>48</v>
@@ -18886,7 +18886,7 @@
         <v>672</v>
       </c>
       <c r="I126" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J126" t="s">
         <v>25</v>
@@ -19799,7 +19799,7 @@
         <v>748</v>
       </c>
       <c r="C142">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D142" t="s">
         <v>70</v>
@@ -19858,7 +19858,7 @@
         <v>753</v>
       </c>
       <c r="C143">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D143" t="s">
         <v>70</v>
@@ -19915,7 +19915,7 @@
         <v>758</v>
       </c>
       <c r="C144">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D144" t="s">
         <v>70</v>
@@ -19974,7 +19974,7 @@
         <v>763</v>
       </c>
       <c r="C145" s="4">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D145" t="s">
         <v>48</v>
@@ -20794,7 +20794,7 @@
         <v>832</v>
       </c>
       <c r="C159">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="D159" t="s">
         <v>48</v>
@@ -20812,7 +20812,7 @@
         <v>835</v>
       </c>
       <c r="I159" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J159" t="s">
         <v>173</v>
@@ -20869,7 +20869,7 @@
         <v>840</v>
       </c>
       <c r="I160" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J160" t="s">
         <v>79</v>
@@ -20985,7 +20985,7 @@
         <v>850</v>
       </c>
       <c r="I162" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J162" t="s">
         <v>60</v>
@@ -21044,7 +21044,7 @@
         <v>855</v>
       </c>
       <c r="I163" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J163" t="s">
         <v>105</v>
@@ -21738,7 +21738,7 @@
         <v>915</v>
       </c>
       <c r="I175" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J175" t="s">
         <v>60</v>
@@ -21779,7 +21779,7 @@
         <v>917</v>
       </c>
       <c r="C176">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="D176" t="s">
         <v>70</v>
@@ -21797,7 +21797,7 @@
         <v>920</v>
       </c>
       <c r="I176" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J176" t="s">
         <v>79</v>
@@ -22011,7 +22011,7 @@
         <v>937</v>
       </c>
       <c r="C180">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D180" t="s">
         <v>70</v>
@@ -22029,7 +22029,7 @@
         <v>940</v>
       </c>
       <c r="I180" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J180" t="s">
         <v>60</v>
@@ -22477,7 +22477,7 @@
         <v>977</v>
       </c>
       <c r="C188">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D188" t="s">
         <v>48</v>
@@ -22495,7 +22495,7 @@
         <v>980</v>
       </c>
       <c r="I188" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J188" t="s">
         <v>43</v>
@@ -24405,7 +24405,7 @@
         <v>1143</v>
       </c>
       <c r="I221" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J221" t="s">
         <v>79</v>
@@ -25278,7 +25278,7 @@
         <v>1218</v>
       </c>
       <c r="I236" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J236" t="s">
         <v>60</v>
@@ -25337,7 +25337,7 @@
         <v>1223</v>
       </c>
       <c r="I237" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J237" t="s">
         <v>79</v>
@@ -25858,7 +25858,7 @@
         <v>593</v>
       </c>
       <c r="I246" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J246" t="s">
         <v>98</v>
@@ -25915,7 +25915,7 @@
         <v>42</v>
       </c>
       <c r="I247" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J247" t="s">
         <v>25</v>
@@ -26528,7 +26528,7 @@
         <v>1321</v>
       </c>
       <c r="C258">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="D258" t="s">
         <v>48</v>
@@ -26660,7 +26660,7 @@
         <v>1334</v>
       </c>
       <c r="I260" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J260" t="s">
         <v>98</v>
@@ -26835,7 +26835,7 @@
         <v>1349</v>
       </c>
       <c r="I263" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J263" t="s">
         <v>173</v>
@@ -27760,7 +27760,7 @@
         <v>1428</v>
       </c>
       <c r="I279" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J279" t="s">
         <v>105</v>
@@ -28051,7 +28051,7 @@
         <v>1453</v>
       </c>
       <c r="I284" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J284" t="s">
         <v>105</v>
@@ -28108,7 +28108,7 @@
         <v>1458</v>
       </c>
       <c r="I285" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J285" t="s">
         <v>25</v>
@@ -28438,7 +28438,7 @@
         <v>1485</v>
       </c>
       <c r="C291">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="D291" t="s">
         <v>48</v>
@@ -28513,7 +28513,7 @@
         <v>1493</v>
       </c>
       <c r="I292" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J292" t="s">
         <v>105</v>
@@ -28804,7 +28804,7 @@
         <v>1518</v>
       </c>
       <c r="I297" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J297" t="s">
         <v>98</v>
@@ -29038,7 +29038,7 @@
         <v>1334</v>
       </c>
       <c r="I301" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J301" t="s">
         <v>43</v>
@@ -29325,7 +29325,7 @@
         <v>1561</v>
       </c>
       <c r="I306" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J306" t="s">
         <v>173</v>
@@ -30251,7 +30251,7 @@
         <v>1640</v>
       </c>
       <c r="I322" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J322" t="s">
         <v>173</v>
@@ -30349,7 +30349,7 @@
         <v>1647</v>
       </c>
       <c r="C324">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="D324" t="s">
         <v>48</v>
@@ -30367,7 +30367,7 @@
         <v>1650</v>
       </c>
       <c r="I324" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J324" t="s">
         <v>86</v>
@@ -30481,7 +30481,7 @@
         <v>1660</v>
       </c>
       <c r="I326" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J326" t="s">
         <v>173</v>
@@ -30540,7 +30540,7 @@
         <v>1665</v>
       </c>
       <c r="I327" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J327" t="s">
         <v>173</v>
@@ -30656,7 +30656,7 @@
         <v>1675</v>
       </c>
       <c r="I329" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J329" t="s">
         <v>173</v>
@@ -30890,7 +30890,7 @@
         <v>1695</v>
       </c>
       <c r="I333" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J333" t="s">
         <v>60</v>
@@ -31507,7 +31507,7 @@
         <v>1746</v>
       </c>
       <c r="C344">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D344" t="s">
         <v>48</v>
@@ -31525,7 +31525,7 @@
         <v>1749</v>
       </c>
       <c r="I344" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J344" t="s">
         <v>105</v>
@@ -31639,7 +31639,7 @@
         <v>1759</v>
       </c>
       <c r="I346" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J346" t="s">
         <v>25</v>
@@ -31757,7 +31757,7 @@
         <v>1769</v>
       </c>
       <c r="I348" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J348" t="s">
         <v>86</v>
@@ -31814,7 +31814,7 @@
         <v>1774</v>
       </c>
       <c r="I349" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="J349" t="s">
         <v>105</v>
@@ -32201,7 +32201,7 @@
         <v>1804</v>
       </c>
       <c r="C356">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="D356" t="s">
         <v>48</v>
@@ -33009,7 +33009,7 @@
         <v>1874</v>
       </c>
       <c r="C370">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="D370" t="s">
         <v>48</v>
@@ -33473,7 +33473,7 @@
         <v>1914</v>
       </c>
       <c r="C378">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="D378" t="s">
         <v>70</v>
@@ -34493,7 +34493,7 @@
         <v>2006</v>
       </c>
       <c r="I396" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="J396" t="s">
         <v>60</v>
@@ -34887,7 +34887,7 @@
         <v>1153</v>
       </c>
       <c r="I403" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="J403" t="s">
         <v>98</v>
@@ -35062,7 +35062,7 @@
         <v>2054</v>
       </c>
       <c r="I406" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="J406" t="s">
         <v>25</v>
@@ -35815,7 +35815,7 @@
         <v>2118</v>
       </c>
       <c r="I419" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="J419" t="s">
         <v>173</v>
@@ -35926,7 +35926,7 @@
         <v>2128</v>
       </c>
       <c r="I421" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="J421" t="s">
         <v>98</v>
@@ -36092,7 +36092,7 @@
         <v>2143</v>
       </c>
       <c r="I424" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="J424" t="s">
         <v>98</v>
@@ -37073,7 +37073,7 @@
         <v>2228</v>
       </c>
       <c r="I441" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="J441" t="s">
         <v>25</v>
@@ -37705,7 +37705,7 @@
         <v>2282</v>
       </c>
       <c r="I452" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="J452" t="s">
         <v>60</v>
@@ -37994,7 +37994,7 @@
         <v>2307</v>
       </c>
       <c r="I457" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="J457" t="s">
         <v>79</v>
@@ -38169,7 +38169,7 @@
         <v>488</v>
       </c>
       <c r="I460" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J460" t="s">
         <v>60</v>
@@ -38210,7 +38210,7 @@
         <v>2323</v>
       </c>
       <c r="C461">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="D461" t="s">
         <v>48</v>
@@ -38267,7 +38267,7 @@
         <v>2328</v>
       </c>
       <c r="C462">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="D462" t="s">
         <v>70</v>
@@ -38324,7 +38324,7 @@
         <v>2333</v>
       </c>
       <c r="C463">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D463" t="s">
         <v>70</v>
@@ -38342,7 +38342,7 @@
         <v>2336</v>
       </c>
       <c r="I463" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J463" t="s">
         <v>25</v>
@@ -38383,7 +38383,7 @@
         <v>2338</v>
       </c>
       <c r="C464">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="D464" t="s">
         <v>48</v>
@@ -38442,7 +38442,7 @@
         <v>2343</v>
       </c>
       <c r="C465">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D465" t="s">
         <v>70</v>
@@ -38460,7 +38460,7 @@
         <v>2346</v>
       </c>
       <c r="I465" t="s">
-        <v>34</v>
+        <v>199</v>
       </c>
       <c r="J465" t="s">
         <v>79</v>
@@ -38500,6 +38500,9 @@
       <c r="B466" t="s">
         <v>2348</v>
       </c>
+      <c r="C466">
+        <v>17</v>
+      </c>
       <c r="D466" t="s">
         <v>70</v>
       </c>
@@ -38612,6 +38615,9 @@
       <c r="B468" t="s">
         <v>2358</v>
       </c>
+      <c r="C468">
+        <v>63</v>
+      </c>
       <c r="D468" t="s">
         <v>70</v>
       </c>
@@ -38668,6 +38674,9 @@
       <c r="B469" t="s">
         <v>2363</v>
       </c>
+      <c r="C469">
+        <v>16</v>
+      </c>
       <c r="D469" t="s">
         <v>48</v>
       </c>
@@ -38725,7 +38734,7 @@
         <v>2368</v>
       </c>
       <c r="C470">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="D470" t="s">
         <v>70</v>
@@ -38743,7 +38752,7 @@
         <v>344</v>
       </c>
       <c r="I470" t="s">
-        <v>34</v>
+        <v>199</v>
       </c>
       <c r="J470" t="s">
         <v>98</v>
@@ -38841,7 +38850,7 @@
         <v>2377</v>
       </c>
       <c r="C472">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="D472" t="s">
         <v>70</v>
@@ -38898,7 +38907,7 @@
         <v>2381</v>
       </c>
       <c r="C473">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="D473" t="s">
         <v>70</v>
@@ -38916,7 +38925,7 @@
         <v>2384</v>
       </c>
       <c r="I473" t="s">
-        <v>34</v>
+        <v>199</v>
       </c>
       <c r="J473" t="s">
         <v>43</v>
@@ -38957,7 +38966,7 @@
         <v>2386</v>
       </c>
       <c r="C474">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D474" t="s">
         <v>70</v>
@@ -39016,7 +39025,7 @@
         <v>2391</v>
       </c>
       <c r="C475">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="D475" t="s">
         <v>70</v>
@@ -39132,7 +39141,7 @@
         <v>2401</v>
       </c>
       <c r="C477">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D477" t="s">
         <v>70</v>
@@ -39189,7 +39198,7 @@
         <v>2406</v>
       </c>
       <c r="C478">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D478" t="s">
         <v>48</v>
@@ -39248,7 +39257,7 @@
         <v>2411</v>
       </c>
       <c r="C479">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D479" t="s">
         <v>70</v>
@@ -39305,7 +39314,7 @@
         <v>2416</v>
       </c>
       <c r="C480">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="D480" t="s">
         <v>70</v>
@@ -39323,7 +39332,7 @@
         <v>2419</v>
       </c>
       <c r="I480" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J480" t="s">
         <v>105</v>
@@ -39362,7 +39371,7 @@
         <v>2421</v>
       </c>
       <c r="C481">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="D481" t="s">
         <v>70</v>
@@ -39380,7 +39389,7 @@
         <v>2424</v>
       </c>
       <c r="I481" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J481" t="s">
         <v>25</v>
@@ -39479,6 +39488,9 @@
       <c r="B483" t="s">
         <v>2431</v>
       </c>
+      <c r="C483">
+        <v>65</v>
+      </c>
       <c r="D483" t="s">
         <v>70</v>
       </c>
@@ -39495,7 +39507,7 @@
         <v>2434</v>
       </c>
       <c r="I483" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J483" t="s">
         <v>25</v>
@@ -39533,6 +39545,9 @@
       <c r="B484" t="s">
         <v>2436</v>
       </c>
+      <c r="C484">
+        <v>65</v>
+      </c>
       <c r="D484" t="s">
         <v>48</v>
       </c>
@@ -39587,6 +39602,9 @@
       <c r="B485" t="s">
         <v>2441</v>
       </c>
+      <c r="C485">
+        <v>65</v>
+      </c>
       <c r="D485" t="s">
         <v>70</v>
       </c>
@@ -39603,7 +39621,7 @@
         <v>2444</v>
       </c>
       <c r="I485" t="s">
-        <v>34</v>
+        <v>199</v>
       </c>
       <c r="J485" t="s">
         <v>60</v>
@@ -39643,6 +39661,9 @@
       <c r="B486" t="s">
         <v>2446</v>
       </c>
+      <c r="C486">
+        <v>65</v>
+      </c>
       <c r="D486" t="s">
         <v>48</v>
       </c>
@@ -39700,7 +39721,7 @@
         <v>2451</v>
       </c>
       <c r="C487">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="D487" t="s">
         <v>70</v>
@@ -39759,7 +39780,7 @@
         <v>2456</v>
       </c>
       <c r="C488">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="D488" t="s">
         <v>70</v>
@@ -39777,7 +39798,7 @@
         <v>2459</v>
       </c>
       <c r="I488" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J488" t="s">
         <v>60</v>
@@ -39818,7 +39839,7 @@
         <v>2461</v>
       </c>
       <c r="C489">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="D489" t="s">
         <v>70</v>
@@ -39875,7 +39896,7 @@
         <v>2466</v>
       </c>
       <c r="C490">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="D490" t="s">
         <v>48</v>
@@ -39893,7 +39914,7 @@
         <v>2469</v>
       </c>
       <c r="I490" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J490" t="s">
         <v>43</v>
@@ -39934,7 +39955,7 @@
         <v>2471</v>
       </c>
       <c r="C491">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D491" t="s">
         <v>70</v>
@@ -40011,7 +40032,7 @@
         <v>2479</v>
       </c>
       <c r="I492" t="s">
-        <v>34</v>
+        <v>199</v>
       </c>
       <c r="J492" t="s">
         <v>86</v>
@@ -40052,7 +40073,7 @@
         <v>2481</v>
       </c>
       <c r="C493">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="D493" t="s">
         <v>70</v>
@@ -40070,7 +40091,7 @@
         <v>2484</v>
       </c>
       <c r="I493" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J493" t="s">
         <v>25</v>
@@ -40168,7 +40189,7 @@
         <v>2491</v>
       </c>
       <c r="C495">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="D495" t="s">
         <v>48</v>
@@ -40186,7 +40207,7 @@
         <v>2494</v>
       </c>
       <c r="I495" t="s">
-        <v>34</v>
+        <v>199</v>
       </c>
       <c r="J495" t="s">
         <v>105</v>
@@ -40225,7 +40246,7 @@
         <v>2496</v>
       </c>
       <c r="C496">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="D496" t="s">
         <v>70</v>
@@ -40243,7 +40264,7 @@
         <v>761</v>
       </c>
       <c r="I496" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J496" t="s">
         <v>79</v>
@@ -40284,7 +40305,7 @@
         <v>2500</v>
       </c>
       <c r="C497">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="D497" t="s">
         <v>48</v>
@@ -40302,7 +40323,7 @@
         <v>2503</v>
       </c>
       <c r="I497" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J497" t="s">
         <v>25</v>
@@ -40343,7 +40364,7 @@
         <v>2505</v>
       </c>
       <c r="C498">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="D498" t="s">
         <v>70</v>
@@ -40361,7 +40382,7 @@
         <v>2508</v>
       </c>
       <c r="I498" t="s">
-        <v>34</v>
+        <v>199</v>
       </c>
       <c r="J498" t="s">
         <v>25</v>
@@ -40400,7 +40421,7 @@
         <v>2510</v>
       </c>
       <c r="C499">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="D499" t="s">
         <v>48</v>
@@ -40418,7 +40439,7 @@
         <v>2513</v>
       </c>
       <c r="I499" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J499" t="s">
         <v>79</v>
@@ -40457,7 +40478,7 @@
         <v>2515</v>
       </c>
       <c r="C500">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="D500" t="s">
         <v>70</v>
@@ -40516,7 +40537,7 @@
         <v>2520</v>
       </c>
       <c r="C501">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="D501" t="s">
         <v>70</v>
@@ -40573,7 +40594,7 @@
         <v>2525</v>
       </c>
       <c r="C502">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D502" t="s">
         <v>70</v>
@@ -40591,7 +40612,7 @@
         <v>2528</v>
       </c>
       <c r="I502" t="s">
-        <v>34</v>
+        <v>199</v>
       </c>
       <c r="J502" t="s">
         <v>79</v>
@@ -40630,7 +40651,7 @@
         <v>2530</v>
       </c>
       <c r="C503">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="D503" t="s">
         <v>70</v>
@@ -40648,7 +40669,7 @@
         <v>2533</v>
       </c>
       <c r="I503" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J503" t="s">
         <v>43</v>
@@ -40689,7 +40710,7 @@
         <v>2535</v>
       </c>
       <c r="C504">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D504" t="s">
         <v>70</v>
@@ -40807,7 +40828,7 @@
         <v>2545</v>
       </c>
       <c r="C506">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="D506" t="s">
         <v>70</v>
@@ -40825,7 +40846,7 @@
         <v>2548</v>
       </c>
       <c r="I506" t="s">
-        <v>34</v>
+        <v>199</v>
       </c>
       <c r="J506" t="s">
         <v>173</v>
@@ -40866,7 +40887,7 @@
         <v>2550</v>
       </c>
       <c r="C507">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="D507" t="s">
         <v>70</v>
@@ -41039,7 +41060,7 @@
         <v>2564</v>
       </c>
       <c r="C510">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="D510" t="s">
         <v>70</v>
@@ -41057,7 +41078,7 @@
         <v>2567</v>
       </c>
       <c r="I510" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J510" t="s">
         <v>25</v>
@@ -41228,7 +41249,7 @@
         <v>51</v>
       </c>
       <c r="I513" t="s">
-        <v>34</v>
+        <v>199</v>
       </c>
       <c r="J513" t="s">
         <v>105</v>
@@ -41285,7 +41306,7 @@
         <v>2586</v>
       </c>
       <c r="I514" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J514" t="s">
         <v>43</v>
@@ -42420,7 +42441,7 @@
         <v>2683</v>
       </c>
       <c r="I534" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J534" t="s">
         <v>173</v>
@@ -42772,7 +42793,7 @@
         <v>2713</v>
       </c>
       <c r="I540" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J540" t="s">
         <v>79</v>
@@ -43000,7 +43021,7 @@
         <v>1193</v>
       </c>
       <c r="I544" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J544" t="s">
         <v>60</v>
@@ -43116,7 +43137,7 @@
         <v>2742</v>
       </c>
       <c r="I546" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J546" t="s">
         <v>173</v>
@@ -43175,7 +43196,7 @@
         <v>2747</v>
       </c>
       <c r="I547" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J547" t="s">
         <v>98</v>
@@ -43698,7 +43719,7 @@
         <v>2792</v>
       </c>
       <c r="I556" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J556" t="s">
         <v>86</v>
@@ -43871,7 +43892,7 @@
         <v>2807</v>
       </c>
       <c r="I559" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J559" t="s">
         <v>25</v>
@@ -43930,7 +43951,7 @@
         <v>2812</v>
       </c>
       <c r="I560" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J560" t="s">
         <v>98</v>
@@ -44100,7 +44121,7 @@
         <v>2826</v>
       </c>
       <c r="I563" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J563" t="s">
         <v>43</v>
@@ -44374,7 +44395,7 @@
         <v>2851</v>
       </c>
       <c r="I568" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J568" t="s">
         <v>60</v>
@@ -44829,7 +44850,7 @@
         <v>2890</v>
       </c>
       <c r="I576" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J576" t="s">
         <v>105</v>
@@ -45474,7 +45495,7 @@
         <v>2945</v>
       </c>
       <c r="I587" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J587" t="s">
         <v>105</v>
@@ -45763,7 +45784,7 @@
         <v>513</v>
       </c>
       <c r="I592" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J592" t="s">
         <v>79</v>
@@ -45822,7 +45843,7 @@
         <v>2974</v>
       </c>
       <c r="I593" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J593" t="s">
         <v>105</v>
@@ -46170,7 +46191,7 @@
         <v>3004</v>
       </c>
       <c r="I599" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J599" t="s">
         <v>43</v>
@@ -47155,7 +47176,7 @@
         <v>3088</v>
       </c>
       <c r="I616" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J616" t="s">
         <v>98</v>
@@ -47788,7 +47809,7 @@
         <v>3142</v>
       </c>
       <c r="I627" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J627" t="s">
         <v>25</v>
@@ -48018,7 +48039,7 @@
         <v>3162</v>
       </c>
       <c r="I631" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J631" t="s">
         <v>60</v>
@@ -48131,7 +48152,7 @@
         <v>3172</v>
       </c>
       <c r="I633" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J633" t="s">
         <v>25</v>
@@ -48242,7 +48263,7 @@
         <v>3182</v>
       </c>
       <c r="I635" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J635" t="s">
         <v>60</v>
@@ -48360,7 +48381,7 @@
         <v>3192</v>
       </c>
       <c r="I637" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J637" t="s">
         <v>98</v>
@@ -48419,7 +48440,7 @@
         <v>3197</v>
       </c>
       <c r="I638" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J638" t="s">
         <v>60</v>
@@ -48651,7 +48672,7 @@
         <v>3217</v>
       </c>
       <c r="I642" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J642" t="s">
         <v>86</v>
@@ -48710,7 +48731,7 @@
         <v>3222</v>
       </c>
       <c r="I643" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
       <c r="J643" t="s">
         <v>105</v>

</xml_diff>